<commit_message>
refactor: word-generator | fix: word-generators & excel-parser
</commit_message>
<xml_diff>
--- a/assets/assets_A/source_1.xlsx
+++ b/assets/assets_A/source_1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2088" yWindow="2088" windowWidth="15396" windowHeight="9648" tabRatio="183" activeTab="1"/>
+    <workbookView xWindow="2088" yWindow="2088" windowWidth="15396" windowHeight="9648" tabRatio="183"/>
   </bookViews>
   <sheets>
     <sheet name="variable" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="157">
   <si>
     <t>E-mail</t>
   </si>
@@ -542,6 +542,12 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>АТ-2022-02</t>
+  </si>
+  <si>
+    <t>AT</t>
   </si>
 </sst>
 </file>
@@ -1103,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z956"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1217,6 +1223,9 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="115.2">
+      <c r="A3" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="B3" s="8" t="s">
         <v>13</v>
       </c>
@@ -1260,6 +1269,9 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4" spans="1:26" ht="86.4">
+      <c r="A4" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="B4" s="8" t="s">
         <v>17</v>
       </c>
@@ -1303,6 +1315,9 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5" spans="1:26" ht="57.6">
+      <c r="A5" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="B5" s="8" t="s">
         <v>19</v>
       </c>
@@ -1346,6 +1361,9 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="187.2">
+      <c r="A6" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
@@ -1389,6 +1407,9 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" ht="43.2">
+      <c r="A7" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="B7" s="8" t="s">
         <v>21</v>
       </c>
@@ -1432,6 +1453,9 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" spans="1:26" ht="57.6">
+      <c r="A8" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="B8" s="8" t="s">
         <v>22</v>
       </c>
@@ -1475,6 +1499,9 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="1:26" ht="72">
+      <c r="A9" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="B9" s="8" t="s">
         <v>23</v>
       </c>
@@ -1518,6 +1545,9 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10" spans="1:26" ht="144">
+      <c r="A10" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="B10" s="8" t="s">
         <v>25</v>
       </c>
@@ -1546,6 +1576,9 @@
       <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:26" ht="43.2">
+      <c r="A11" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="B11" s="8" t="s">
         <v>27</v>
       </c>
@@ -1574,6 +1607,9 @@
       <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:26" ht="43.2">
+      <c r="A12" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="B12" s="8" t="s">
         <v>30</v>
       </c>
@@ -1602,6 +1638,9 @@
       <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:26" ht="72">
+      <c r="A13" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="B13" s="8" t="s">
         <v>32</v>
       </c>
@@ -1629,7 +1668,35 @@
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:26" ht="83.4" customHeight="1">
+      <c r="A14" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="16">
+        <v>1</v>
+      </c>
+      <c r="F14" s="14">
+        <v>10000</v>
+      </c>
+      <c r="G14" s="15">
+        <v>44563</v>
+      </c>
+      <c r="H14" s="15">
+        <v>44593</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="16" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
@@ -2588,7 +2655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH949"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>

</xml_diff>